<commit_message>
Se agregaron cambios solicitados, pendiente incorporar reporte de bug
</commit_message>
<xml_diff>
--- a/src/public/assets/plantilla/plantillaExpedientes.xlsx
+++ b/src/public/assets/plantilla/plantillaExpedientes.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Asus\Documents\Cursos\pugnode - copia - copia\src\public\assets\plantilla\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0561B7A5-7E62-4512-876B-7194B82A775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="intrucciones"/>
-    <sheet r:id="rId2" sheetId="2" name="datos"/>
+    <sheet name="intrucciones" sheetId="1" r:id="rId1"/>
+    <sheet name="datos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Numero Expediente</t>
   </si>
@@ -23,9 +29,6 @@
     <t>Nombre Expediente</t>
   </si>
   <si>
-    <t>Numero Serie</t>
-  </si>
-  <si>
     <t>Nombre Serie</t>
   </si>
   <si>
@@ -38,9 +41,6 @@
     <t>Caja</t>
   </si>
   <si>
-    <t>Tipo documento</t>
-  </si>
-  <si>
     <t>Estado Organizacional</t>
   </si>
   <si>
@@ -53,9 +53,6 @@
     <t>10F</t>
   </si>
   <si>
-    <t>Contrato</t>
-  </si>
-  <si>
     <t>Aerodromo Saravena</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>40D</t>
   </si>
   <si>
-    <t>Aerodromo</t>
-  </si>
-  <si>
     <t>Jhoan  Zamudio</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>52F</t>
   </si>
   <si>
-    <t>Resolucion</t>
-  </si>
-  <si>
     <t>Aerodromo Barbosa</t>
   </si>
   <si>
@@ -104,22 +95,13 @@
     <t>Número de expediente</t>
   </si>
   <si>
-    <t>Número de serie</t>
-  </si>
-  <si>
     <t>Nombre de serie</t>
   </si>
   <si>
-    <t>Tipo Documento</t>
-  </si>
-  <si>
     <t>El nombre expediente contine algún dato especifico sobre el documento, el cual puede ser el nombre de la persona, a la cual pertenece el expediente, el nombre de la resolución, el nombre del aeródromo ETC.</t>
   </si>
   <si>
     <t>Debe contener el número de identificación de ese expediente.</t>
-  </si>
-  <si>
-    <t>Debe contener el numero de serie documental a la cual pertenece este expediente.</t>
   </si>
   <si>
     <t>Debe contener el no,bre de la serie a la cual pertenece el expediente.</t>
@@ -176,32 +158,6 @@
   </si>
   <si>
     <r>
-      <t>Se refiere a la clasificación de este expediente, en las cuales tenemos: c</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ontrato, resolucion, historia clinica, historia laboral, aerodromo,licencia, accidente aereo, otro</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Por favor, en lo posible agregar alguno de estos tipos de documento.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Se réfiere a la organización del expediente, si ya encuentra úbicado y organizado de forma permanente o si se encuentra desubicado o sin organizar aun. Si el expediente ya se encuentra en estado organizado solo debes color un</t>
     </r>
     <r>
@@ -243,22 +199,12 @@
   <si>
     <t>Ejemplo para la Inserción de datos.</t>
   </si>
-  <si>
-    <t>Accidente avianca 1954</t>
-  </si>
-  <si>
-    <t>Accidentes Aereos</t>
-  </si>
-  <si>
-    <t>accidente aereo</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,7 +226,7 @@
     </font>
     <font>
       <sz val="22"/>
-      <color rgb="FFed7d31"/>
+      <color rgb="FFED7D31"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -292,15 +238,38 @@
     </font>
     <font>
       <sz val="20"/>
-      <color rgb="FFed7d31"/>
+      <color rgb="FFED7D31"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="26"/>
-      <color rgb="FF2e75b6"/>
+      <color rgb="FF2E75B6"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -312,17 +281,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFa9d18e"/>
+        <fgColor rgb="FFA9D18E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf8cbad"/>
+        <fgColor rgb="FFF8CBAD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -357,10 +326,10 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -384,110 +353,108 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -498,10 +465,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -539,71 +506,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -631,7 +598,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -654,11 +621,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -667,13 +634,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -683,7 +650,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -692,7 +659,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -701,7 +668,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -709,10 +676,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -777,265 +744,246 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="30" width="42.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="31" width="32.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="30" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="31" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="31" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="30" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="30" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="29.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="30" width="51.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="42.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.88671875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.6640625" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33">
+    <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" s="16" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="23.25">
-      <c r="A3" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="F4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="18" t="s">
+      <c r="H4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" s="16" customFormat="1" ht="27.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="115.5" customFormat="1" s="19">
-      <c r="A4" s="20" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" s="16" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A10" s="12"/>
+      <c r="B10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="27.375" customFormat="1" s="19">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="31.5" customFormat="1" s="19">
-      <c r="A7" s="22"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="27">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="15"/>
-      <c r="B10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="H11" s="6"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>7895462</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="4">
-        <v>5500</v>
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="E12" s="4">
+        <v>25</v>
       </c>
       <c r="F12" s="4">
-        <v>25</v>
-      </c>
-      <c r="G12" s="4">
         <v>50</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="7">
+      <c r="G12" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>25455463</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4">
         <v>4000</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F13" s="4">
         <v>10</v>
       </c>
       <c r="G13" s="4">
-        <v>50</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="7">
         <v>0</v>
       </c>
+      <c r="I13"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1044,213 +992,178 @@
     <mergeCell ref="B10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="9" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="24.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="16.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    </row>
+    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>7895462</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4">
-        <v>8000</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
+      <c r="E2" s="4">
+        <v>25</v>
       </c>
       <c r="F2" s="4">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4">
         <v>50</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="7">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>7895463</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4">
-        <v>4000</v>
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="E3" s="4">
+        <v>10</v>
       </c>
       <c r="F3" s="4">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4">
         <v>50</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="7">
+      <c r="G3" s="7">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>7895465</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="4">
-        <v>8000</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>20</v>
       </c>
       <c r="F4" s="4">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4">
         <v>50</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="G4" s="7">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>7895467</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4000</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="E5" s="4">
+        <v>12</v>
       </c>
       <c r="F5" s="4">
-        <v>12</v>
-      </c>
-      <c r="G5" s="4">
         <v>50</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="G5" s="7">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="8"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    </row>
+    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>78954610</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4">
-        <v>7200</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
       </c>
       <c r="F7" s="4">
-        <v>5</v>
-      </c>
-      <c r="G7" s="4">
         <v>50</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="7">
+      <c r="G7" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>